<commit_message>
latest metadata list (#43)
</commit_message>
<xml_diff>
--- a/assets/metadata/latest/PancDB_ATAC-seq_metadata_2022-06-15.xlsx
+++ b/assets/metadata/latest/PancDB_ATAC-seq_metadata_2022-06-15.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25003"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisabetta\Documents\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisabetta\Documents\tmp\PancDB_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_E4E2EC1DDB51A145A4A518DB1D76D3EA4E186FAC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32490" windowHeight="16965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33810" windowHeight="16665"/>
   </bookViews>
   <sheets>
     <sheet name="PancDB_ATAC-seq_metadata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'PancDB_ATAC-seq_metadata'!$A$1:$P$50</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -324,9 +326,6 @@
     <t>HPAP-035</t>
   </si>
   <si>
-    <t>Islet acinar cells</t>
-  </si>
-  <si>
     <t>FGC2083</t>
   </si>
   <si>
@@ -342,9 +341,6 @@
     <t>50x50</t>
   </si>
   <si>
-    <t>HPAP-035_acinar_FGC2083_s_8_1_AGGCAGAA.fastq.gz,HPAP-035_acinar_FGC2083_s_8_2_AGGCAGAA.fastq.gz</t>
-  </si>
-  <si>
     <t>HPAP-035_alpha_FGC2083_s_8_1_TAAGGCGA.fastq.gz,HPAP-035_alpha_FGC2083_s_8_2_TAAGGCGA.fastq.gz</t>
   </si>
   <si>
@@ -489,9 +485,6 @@
     <t>50x50;50x50;50x50</t>
   </si>
   <si>
-    <t>HPAP-063_acinar_FGC2163_s_1_1_TAGGCATG.fastq.gz,HPAP-063_acinar_FGC2163_s_1_2_TAGGCATG.fastq.gz;HPAP-063_acinar_FGC2163_s_2_1_TAGGCATG.fastq.gz,HPAP-063_acinar_FGC2163_s_2_2_TAGGCATG.fastq.gz;HPAP-063_acinar_FGC2252_s_2_1_TAGGCATG.fastq.gz,HPAP-063_acinar_FGC2252_s_2_2_TAGGCATG.fastq.gz</t>
-  </si>
-  <si>
     <t>99252;99252;103199</t>
   </si>
   <si>
@@ -513,18 +506,12 @@
     <t>99260;99260;103204</t>
   </si>
   <si>
-    <t>HPAP-066_acinar_FGC2163_s_1_1_GTAGAGGA.fastq.gz,HPAP-066_acinar_FGC2163_s_1_2_GTAGAGGA.fastq.gz;HPAP-066_acinar_FGC2163_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_acinar_FGC2163_s_2_2_GTAGAGGA.fastq.gz;HPAP-066_acinar_FGC2252_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_acinar_FGC2252_s_2_2_GTAGAGGA.fastq.gz</t>
-  </si>
-  <si>
     <t>HPAP-067</t>
   </si>
   <si>
     <t>99263;99263;103206</t>
   </si>
   <si>
-    <t>HPAP-067_acinar_FGC2163_s_1_1_TGGATCTG.fastq.gz,HPAP-067_acinar_FGC2163_s_1_2_TGGATCTG.fastq.gz;HPAP-067_acinar_FGC2163_s_2_1_TGGATCTG.fastq.gz,HPAP-067_acinar_FGC2163_s_2_2_TGGATCTG.fastq.gz;HPAP-067_acinar_FGC2252_s_2_1_TGGATCTG.fastq.gz,HPAP-067_acinar_FGC2252_s_2_2_TGGATCTG.fastq.gz</t>
-  </si>
-  <si>
     <t>HPAP-069</t>
   </si>
   <si>
@@ -556,13 +543,28 @@
   </si>
   <si>
     <t>HPAP-077_beta_FGC2229_s_2_1_GTCGTGAT.fastq.gz,HPAP-077_beta_FGC2229_s_2_2_GTCGTGAT.fastq.gz</t>
+  </si>
+  <si>
+    <t>Islet exocrine cells</t>
+  </si>
+  <si>
+    <t>HPAP-067_exocrine_FGC2163_s_1_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_1_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2163_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_2_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2252_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2252_s_2_2_TGGATCTG.fastq.gz</t>
+  </si>
+  <si>
+    <t>HPAP-035_exocrine_FGC2083_s_8_1_AGGCAGAA.fastq.gz,HPAP-035_exocrine_FGC2083_s_8_2_AGGCAGAA.fastq.gz</t>
+  </si>
+  <si>
+    <t>HPAP-063_exocrine_FGC2163_s_1_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_1_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2163_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_2_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2252_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2252_s_2_2_TAGGCATG.fastq.gz</t>
+  </si>
+  <si>
+    <t>HPAP-066_exocrine_FGC2163_s_1_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_1_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2163_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_2_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2252_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2252_s_2_2_GTAGAGGA.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1362,14 +1364,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="D45" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1389,7 +1391,7 @@
     <col min="16" max="16" width="176.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1439,7 +1441,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1515,7 +1517,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1553,7 +1555,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1591,7 +1593,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1629,7 +1631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1667,7 +1669,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1705,7 +1707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1743,7 +1745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1819,7 +1821,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1854,7 +1856,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1889,7 +1891,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1924,7 +1926,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1959,7 +1961,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -1994,7 +1996,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -2029,7 +2031,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2064,7 +2066,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2099,7 +2101,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -2134,7 +2136,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -2169,7 +2171,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -2204,7 +2206,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -2239,7 +2241,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -2250,31 +2252,31 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>170</v>
       </c>
       <c r="E24">
         <v>92020</v>
       </c>
       <c r="H24" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" t="s">
         <v>98</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>99</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>100</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>101</v>
       </c>
-      <c r="L24" t="s">
-        <v>102</v>
-      </c>
       <c r="M24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -2291,25 +2293,25 @@
         <v>92018</v>
       </c>
       <c r="H25" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" t="s">
         <v>98</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>99</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>100</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>101</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>102</v>
       </c>
-      <c r="M25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -2326,27 +2328,27 @@
         <v>92019</v>
       </c>
       <c r="H26" t="s">
+        <v>97</v>
+      </c>
+      <c r="I26" t="s">
         <v>98</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>99</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>100</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>101</v>
       </c>
-      <c r="L26" t="s">
-        <v>102</v>
-      </c>
       <c r="M26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
@@ -2358,7 +2360,7 @@
         <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H27" t="s">
         <v>55</v>
@@ -2376,12 +2378,12 @@
         <v>59</v>
       </c>
       <c r="M27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
@@ -2396,27 +2398,27 @@
         <v>92021</v>
       </c>
       <c r="H28" t="s">
+        <v>97</v>
+      </c>
+      <c r="I28" t="s">
         <v>98</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>99</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>100</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>101</v>
       </c>
-      <c r="L28" t="s">
-        <v>102</v>
-      </c>
       <c r="M28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -2428,7 +2430,7 @@
         <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H29" t="s">
         <v>55</v>
@@ -2446,12 +2448,12 @@
         <v>59</v>
       </c>
       <c r="M29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B30" t="s">
         <v>17</v>
@@ -2463,7 +2465,7 @@
         <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H30" t="s">
         <v>55</v>
@@ -2481,12 +2483,12 @@
         <v>59</v>
       </c>
       <c r="M30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
@@ -2501,27 +2503,27 @@
         <v>92024</v>
       </c>
       <c r="H31" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" t="s">
         <v>98</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>99</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>100</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>101</v>
       </c>
-      <c r="L31" t="s">
-        <v>102</v>
-      </c>
       <c r="M31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -2536,27 +2538,27 @@
         <v>92025</v>
       </c>
       <c r="H32" t="s">
+        <v>97</v>
+      </c>
+      <c r="I32" t="s">
         <v>98</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>99</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>100</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>101</v>
       </c>
-      <c r="L32" t="s">
-        <v>102</v>
-      </c>
       <c r="M32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
@@ -2568,7 +2570,7 @@
         <v>46</v>
       </c>
       <c r="E33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H33" t="s">
         <v>66</v>
@@ -2586,12 +2588,12 @@
         <v>70</v>
       </c>
       <c r="M33" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
         <v>17</v>
@@ -2603,7 +2605,7 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H34" t="s">
         <v>66</v>
@@ -2621,12 +2623,12 @@
         <v>70</v>
       </c>
       <c r="M34" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -2638,7 +2640,7 @@
         <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H35" t="s">
         <v>66</v>
@@ -2656,12 +2658,12 @@
         <v>70</v>
       </c>
       <c r="M35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
@@ -2673,7 +2675,7 @@
         <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H36" t="s">
         <v>55</v>
@@ -2691,12 +2693,12 @@
         <v>59</v>
       </c>
       <c r="M36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B37" t="s">
         <v>17</v>
@@ -2708,7 +2710,7 @@
         <v>46</v>
       </c>
       <c r="E37" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H37" t="s">
         <v>55</v>
@@ -2726,12 +2728,12 @@
         <v>59</v>
       </c>
       <c r="M37" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
         <v>17</v>
@@ -2743,7 +2745,7 @@
         <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H38" t="s">
         <v>55</v>
@@ -2761,12 +2763,12 @@
         <v>59</v>
       </c>
       <c r="M38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
         <v>17</v>
@@ -2778,30 +2780,30 @@
         <v>19</v>
       </c>
       <c r="E39" t="s">
+        <v>134</v>
+      </c>
+      <c r="H39" t="s">
+        <v>135</v>
+      </c>
+      <c r="I39" t="s">
         <v>136</v>
       </c>
-      <c r="H39" t="s">
+      <c r="J39" t="s">
         <v>137</v>
       </c>
-      <c r="I39" t="s">
+      <c r="K39" t="s">
         <v>138</v>
       </c>
-      <c r="J39" t="s">
+      <c r="L39" t="s">
         <v>139</v>
       </c>
-      <c r="K39" t="s">
+      <c r="M39" t="s">
         <v>140</v>
       </c>
-      <c r="L39" t="s">
-        <v>141</v>
-      </c>
-      <c r="M39" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
@@ -2813,65 +2815,65 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
+        <v>141</v>
+      </c>
+      <c r="H40" t="s">
+        <v>135</v>
+      </c>
+      <c r="I40" t="s">
+        <v>136</v>
+      </c>
+      <c r="J40" t="s">
+        <v>137</v>
+      </c>
+      <c r="K40" t="s">
+        <v>138</v>
+      </c>
+      <c r="L40" t="s">
+        <v>139</v>
+      </c>
+      <c r="M40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>143</v>
       </c>
-      <c r="H40" t="s">
-        <v>137</v>
-      </c>
-      <c r="I40" t="s">
-        <v>138</v>
-      </c>
-      <c r="J40" t="s">
-        <v>139</v>
-      </c>
-      <c r="K40" t="s">
-        <v>140</v>
-      </c>
-      <c r="L40" t="s">
-        <v>141</v>
-      </c>
-      <c r="M40" t="s">
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" t="s">
+      <c r="H41" t="s">
         <v>145</v>
       </c>
-      <c r="B41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" t="s">
-        <v>97</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="I41" t="s">
         <v>146</v>
       </c>
-      <c r="H41" t="s">
+      <c r="J41" t="s">
         <v>147</v>
       </c>
-      <c r="I41" t="s">
+      <c r="K41" t="s">
         <v>148</v>
       </c>
-      <c r="J41" t="s">
+      <c r="L41" t="s">
         <v>149</v>
       </c>
-      <c r="K41" t="s">
-        <v>150</v>
-      </c>
-      <c r="L41" t="s">
-        <v>151</v>
-      </c>
       <c r="M41" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B42" t="s">
         <v>17</v>
@@ -2883,30 +2885,30 @@
         <v>19</v>
       </c>
       <c r="E42" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H42" t="s">
+        <v>145</v>
+      </c>
+      <c r="I42" t="s">
+        <v>146</v>
+      </c>
+      <c r="J42" t="s">
         <v>147</v>
       </c>
-      <c r="I42" t="s">
+      <c r="K42" t="s">
         <v>148</v>
       </c>
-      <c r="J42" t="s">
+      <c r="L42" t="s">
         <v>149</v>
       </c>
-      <c r="K42" t="s">
-        <v>150</v>
-      </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
         <v>151</v>
       </c>
-      <c r="M42" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B43" t="s">
         <v>17</v>
@@ -2918,100 +2920,100 @@
         <v>19</v>
       </c>
       <c r="E43" t="s">
+        <v>153</v>
+      </c>
+      <c r="H43" t="s">
+        <v>145</v>
+      </c>
+      <c r="I43" t="s">
+        <v>146</v>
+      </c>
+      <c r="J43" t="s">
+        <v>147</v>
+      </c>
+      <c r="K43" t="s">
+        <v>148</v>
+      </c>
+      <c r="L43" t="s">
+        <v>149</v>
+      </c>
+      <c r="M43" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" t="s">
+        <v>170</v>
+      </c>
+      <c r="E44" t="s">
         <v>156</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
+        <v>145</v>
+      </c>
+      <c r="I44" t="s">
+        <v>146</v>
+      </c>
+      <c r="J44" t="s">
         <v>147</v>
       </c>
-      <c r="I43" t="s">
+      <c r="K44" t="s">
         <v>148</v>
       </c>
-      <c r="J43" t="s">
+      <c r="L44" t="s">
         <v>149</v>
       </c>
-      <c r="K43" t="s">
-        <v>150</v>
-      </c>
-      <c r="L43" t="s">
-        <v>151</v>
-      </c>
-      <c r="M43" t="s">
+      <c r="M44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" t="s">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>170</v>
+      </c>
+      <c r="E45" t="s">
         <v>158</v>
       </c>
-      <c r="B44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" t="s">
-        <v>97</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="H45" t="s">
+        <v>145</v>
+      </c>
+      <c r="I45" t="s">
+        <v>146</v>
+      </c>
+      <c r="J45" t="s">
+        <v>147</v>
+      </c>
+      <c r="K45" t="s">
+        <v>148</v>
+      </c>
+      <c r="L45" t="s">
+        <v>149</v>
+      </c>
+      <c r="M45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>159</v>
-      </c>
-      <c r="H44" t="s">
-        <v>147</v>
-      </c>
-      <c r="I44" t="s">
-        <v>148</v>
-      </c>
-      <c r="J44" t="s">
-        <v>149</v>
-      </c>
-      <c r="K44" t="s">
-        <v>150</v>
-      </c>
-      <c r="L44" t="s">
-        <v>151</v>
-      </c>
-      <c r="M44" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" t="s">
-        <v>161</v>
-      </c>
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" t="s">
-        <v>97</v>
-      </c>
-      <c r="E45" t="s">
-        <v>162</v>
-      </c>
-      <c r="H45" t="s">
-        <v>147</v>
-      </c>
-      <c r="I45" t="s">
-        <v>148</v>
-      </c>
-      <c r="J45" t="s">
-        <v>149</v>
-      </c>
-      <c r="K45" t="s">
-        <v>150</v>
-      </c>
-      <c r="L45" t="s">
-        <v>151</v>
-      </c>
-      <c r="M45" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46" t="s">
-        <v>164</v>
       </c>
       <c r="B46" t="s">
         <v>17</v>
@@ -3026,27 +3028,27 @@
         <v>101012</v>
       </c>
       <c r="H46" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J46" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K46" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="L46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M46" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B47" t="s">
         <v>17</v>
@@ -3061,27 +3063,27 @@
         <v>101013</v>
       </c>
       <c r="H47" t="s">
+        <v>160</v>
+      </c>
+      <c r="I47" t="s">
+        <v>98</v>
+      </c>
+      <c r="J47" t="s">
+        <v>161</v>
+      </c>
+      <c r="K47" t="s">
+        <v>162</v>
+      </c>
+      <c r="L47" t="s">
+        <v>101</v>
+      </c>
+      <c r="M47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>165</v>
-      </c>
-      <c r="I47" t="s">
-        <v>99</v>
-      </c>
-      <c r="J47" t="s">
-        <v>166</v>
-      </c>
-      <c r="K47" t="s">
-        <v>167</v>
-      </c>
-      <c r="L47" t="s">
-        <v>102</v>
-      </c>
-      <c r="M47" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" t="s">
-        <v>170</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
@@ -3096,27 +3098,27 @@
         <v>101015</v>
       </c>
       <c r="H48" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J48" t="s">
+        <v>161</v>
+      </c>
+      <c r="K48" t="s">
+        <v>162</v>
+      </c>
+      <c r="L48" t="s">
+        <v>101</v>
+      </c>
+      <c r="M48" t="s">
         <v>166</v>
       </c>
-      <c r="K48" t="s">
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>167</v>
-      </c>
-      <c r="L48" t="s">
-        <v>102</v>
-      </c>
-      <c r="M48" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" t="s">
-        <v>172</v>
       </c>
       <c r="B49" t="s">
         <v>17</v>
@@ -3131,27 +3133,27 @@
         <v>101023</v>
       </c>
       <c r="H49" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J49" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K49" t="s">
+        <v>162</v>
+      </c>
+      <c r="L49" t="s">
+        <v>101</v>
+      </c>
+      <c r="M49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>167</v>
-      </c>
-      <c r="L49" t="s">
-        <v>102</v>
-      </c>
-      <c r="M49" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50" t="s">
-        <v>172</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
@@ -3166,26 +3168,27 @@
         <v>101024</v>
       </c>
       <c r="H50" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J50" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K50" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="L50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M50" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:P50">
+  <autoFilter ref="A1:P50"/>
+  <sortState ref="A12:P50">
     <sortCondition ref="A12:A50"/>
     <sortCondition ref="D12:D50"/>
   </sortState>

</xml_diff>

<commit_message>
adding updated metadata files
</commit_message>
<xml_diff>
--- a/assets/metadata/latest/PancDB_ATAC-seq_metadata_2022-06-15.xlsx
+++ b/assets/metadata/latest/PancDB_ATAC-seq_metadata_2022-06-15.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisabetta\Documents\tmp\PancDB_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilanjanasamanta/Library/CloudStorage/Box-Box/HPAP-IBI/Pancdb-Metadata/current_v3.1.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD0E7E0-FDAA-F943-8ED8-7D1989566827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33810" windowHeight="16665"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33820" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PancDB_ATAC-seq_metadata" sheetId="1" r:id="rId1"/>
@@ -19,14 +20,8 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -326,6 +321,9 @@
     <t>HPAP-035</t>
   </si>
   <si>
+    <t>Islet exocrine cells</t>
+  </si>
+  <si>
     <t>FGC2083</t>
   </si>
   <si>
@@ -341,6 +339,9 @@
     <t>50x50</t>
   </si>
   <si>
+    <t>HPAP-035_exocrine_FGC2083_s_8_1_AGGCAGAA.fastq.gz,HPAP-035_exocrine_FGC2083_s_8_2_AGGCAGAA.fastq.gz</t>
+  </si>
+  <si>
     <t>HPAP-035_alpha_FGC2083_s_8_1_TAAGGCGA.fastq.gz,HPAP-035_alpha_FGC2083_s_8_2_TAAGGCGA.fastq.gz</t>
   </si>
   <si>
@@ -485,6 +486,9 @@
     <t>50x50;50x50;50x50</t>
   </si>
   <si>
+    <t>HPAP-063_exocrine_FGC2163_s_1_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_1_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2163_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_2_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2252_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2252_s_2_2_TAGGCATG.fastq.gz</t>
+  </si>
+  <si>
     <t>99252;99252;103199</t>
   </si>
   <si>
@@ -506,12 +510,18 @@
     <t>99260;99260;103204</t>
   </si>
   <si>
+    <t>HPAP-066_exocrine_FGC2163_s_1_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_1_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2163_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_2_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2252_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2252_s_2_2_GTAGAGGA.fastq.gz</t>
+  </si>
+  <si>
     <t>HPAP-067</t>
   </si>
   <si>
     <t>99263;99263;103206</t>
   </si>
   <si>
+    <t>HPAP-067_exocrine_FGC2163_s_1_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_1_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2163_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_2_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2252_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2252_s_2_2_TGGATCTG.fastq.gz</t>
+  </si>
+  <si>
     <t>HPAP-069</t>
   </si>
   <si>
@@ -543,27 +553,12 @@
   </si>
   <si>
     <t>HPAP-077_beta_FGC2229_s_2_1_GTCGTGAT.fastq.gz,HPAP-077_beta_FGC2229_s_2_2_GTCGTGAT.fastq.gz</t>
-  </si>
-  <si>
-    <t>Islet exocrine cells</t>
-  </si>
-  <si>
-    <t>HPAP-067_exocrine_FGC2163_s_1_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_1_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2163_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_2_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2252_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2252_s_2_2_TGGATCTG.fastq.gz</t>
-  </si>
-  <si>
-    <t>HPAP-035_exocrine_FGC2083_s_8_1_AGGCAGAA.fastq.gz,HPAP-035_exocrine_FGC2083_s_8_2_AGGCAGAA.fastq.gz</t>
-  </si>
-  <si>
-    <t>HPAP-063_exocrine_FGC2163_s_1_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_1_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2163_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_2_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2252_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2252_s_2_2_TAGGCATG.fastq.gz</t>
-  </si>
-  <si>
-    <t>HPAP-066_exocrine_FGC2163_s_1_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_1_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2163_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_2_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2252_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2252_s_2_2_GTAGAGGA.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1364,34 +1359,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="83" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="176.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="176.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1441,7 +1436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1479,9 +1474,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1490,7 +1485,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -1505,10 +1500,10 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="O3" t="s">
         <v>26</v>
@@ -1517,9 +1512,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -1543,10 +1538,10 @@
         <v>23</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O4" t="s">
         <v>26</v>
@@ -1555,9 +1550,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1581,10 +1576,10 @@
         <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O5" t="s">
         <v>26</v>
@@ -1593,9 +1588,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1604,7 +1599,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -1619,10 +1614,10 @@
         <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="N6" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="O6" t="s">
         <v>26</v>
@@ -1631,9 +1626,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -1657,10 +1652,10 @@
         <v>23</v>
       </c>
       <c r="M7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O7" t="s">
         <v>26</v>
@@ -1669,9 +1664,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1695,10 +1690,10 @@
         <v>23</v>
       </c>
       <c r="M8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O8" t="s">
         <v>26</v>
@@ -1707,9 +1702,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1718,36 +1713,33 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="L9" t="s">
+        <v>59</v>
       </c>
       <c r="M9" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1756,36 +1748,33 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="L10" t="s">
+        <v>59</v>
       </c>
       <c r="M10" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10" t="s">
-        <v>50</v>
-      </c>
-      <c r="O10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -1794,36 +1783,33 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" t="s">
+        <v>66</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="K11" t="s">
-        <v>23</v>
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
+        <v>70</v>
       </c>
       <c r="M11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -1835,30 +1821,30 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="M12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -1869,31 +1855,34 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" t="s">
-        <v>55</v>
+      <c r="F13" t="s">
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="K13" t="s">
-        <v>58</v>
-      </c>
-      <c r="L13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="N13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1905,7 +1894,7 @@
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
         <v>66</v>
@@ -1923,12 +1912,12 @@
         <v>70</v>
       </c>
       <c r="M14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -1940,7 +1929,7 @@
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
         <v>66</v>
@@ -1958,12 +1947,12 @@
         <v>70</v>
       </c>
       <c r="M15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1974,31 +1963,34 @@
       <c r="D16" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" t="s">
-        <v>66</v>
+      <c r="F16" t="s">
+        <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="J16" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="K16" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="M16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="N16" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -2007,31 +1999,34 @@
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" t="s">
-        <v>66</v>
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="K17" t="s">
-        <v>69</v>
-      </c>
-      <c r="L17" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="M17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="N17" t="s">
+        <v>52</v>
+      </c>
+      <c r="O17" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2066,7 +2061,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2101,7 +2096,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -2136,7 +2131,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -2171,7 +2166,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -2206,7 +2201,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -2241,7 +2236,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -2252,31 +2247,31 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
+        <v>97</v>
       </c>
       <c r="E24">
         <v>92020</v>
       </c>
       <c r="H24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M24" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -2293,25 +2288,25 @@
         <v>92018</v>
       </c>
       <c r="H25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -2328,27 +2323,27 @@
         <v>92019</v>
       </c>
       <c r="H26" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
@@ -2360,7 +2355,7 @@
         <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H27" t="s">
         <v>55</v>
@@ -2378,12 +2373,12 @@
         <v>59</v>
       </c>
       <c r="M27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
@@ -2398,27 +2393,27 @@
         <v>92021</v>
       </c>
       <c r="H28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -2430,7 +2425,7 @@
         <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H29" t="s">
         <v>55</v>
@@ -2448,12 +2443,12 @@
         <v>59</v>
       </c>
       <c r="M29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>109</v>
       </c>
       <c r="B30" t="s">
         <v>17</v>
@@ -2465,7 +2460,7 @@
         <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H30" t="s">
         <v>55</v>
@@ -2483,12 +2478,12 @@
         <v>59</v>
       </c>
       <c r="M30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
@@ -2503,27 +2498,27 @@
         <v>92024</v>
       </c>
       <c r="H31" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I31" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M31" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -2538,27 +2533,27 @@
         <v>92025</v>
       </c>
       <c r="H32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K32" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
@@ -2570,7 +2565,7 @@
         <v>46</v>
       </c>
       <c r="E33" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H33" t="s">
         <v>66</v>
@@ -2588,12 +2583,12 @@
         <v>70</v>
       </c>
       <c r="M33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
         <v>17</v>
@@ -2605,7 +2600,7 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H34" t="s">
         <v>66</v>
@@ -2623,12 +2618,12 @@
         <v>70</v>
       </c>
       <c r="M34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>120</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -2640,7 +2635,7 @@
         <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H35" t="s">
         <v>66</v>
@@ -2658,12 +2653,12 @@
         <v>70</v>
       </c>
       <c r="M35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
@@ -2675,7 +2670,7 @@
         <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H36" t="s">
         <v>55</v>
@@ -2693,12 +2688,12 @@
         <v>59</v>
       </c>
       <c r="M36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>125</v>
       </c>
       <c r="B37" t="s">
         <v>17</v>
@@ -2710,7 +2705,7 @@
         <v>46</v>
       </c>
       <c r="E37" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H37" t="s">
         <v>55</v>
@@ -2728,12 +2723,12 @@
         <v>59</v>
       </c>
       <c r="M37" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
         <v>17</v>
@@ -2745,7 +2740,7 @@
         <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H38" t="s">
         <v>55</v>
@@ -2763,12 +2758,12 @@
         <v>59</v>
       </c>
       <c r="M38" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B39" t="s">
         <v>17</v>
@@ -2780,30 +2775,30 @@
         <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H39" t="s">
+        <v>137</v>
+      </c>
+      <c r="I39" t="s">
+        <v>138</v>
+      </c>
+      <c r="J39" t="s">
+        <v>139</v>
+      </c>
+      <c r="K39" t="s">
+        <v>140</v>
+      </c>
+      <c r="L39" t="s">
+        <v>141</v>
+      </c>
+      <c r="M39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>135</v>
-      </c>
-      <c r="I39" t="s">
-        <v>136</v>
-      </c>
-      <c r="J39" t="s">
-        <v>137</v>
-      </c>
-      <c r="K39" t="s">
-        <v>138</v>
-      </c>
-      <c r="L39" t="s">
-        <v>139</v>
-      </c>
-      <c r="M39" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>133</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
@@ -2815,30 +2810,30 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
+        <v>143</v>
+      </c>
+      <c r="H40" t="s">
+        <v>137</v>
+      </c>
+      <c r="I40" t="s">
+        <v>138</v>
+      </c>
+      <c r="J40" t="s">
+        <v>139</v>
+      </c>
+      <c r="K40" t="s">
+        <v>140</v>
+      </c>
+      <c r="L40" t="s">
         <v>141</v>
       </c>
-      <c r="H40" t="s">
-        <v>135</v>
-      </c>
-      <c r="I40" t="s">
-        <v>136</v>
-      </c>
-      <c r="J40" t="s">
-        <v>137</v>
-      </c>
-      <c r="K40" t="s">
-        <v>138</v>
-      </c>
-      <c r="L40" t="s">
-        <v>139</v>
-      </c>
       <c r="M40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
         <v>17</v>
@@ -2847,33 +2842,33 @@
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>170</v>
+        <v>97</v>
       </c>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H41" t="s">
+        <v>147</v>
+      </c>
+      <c r="I41" t="s">
+        <v>148</v>
+      </c>
+      <c r="J41" t="s">
+        <v>149</v>
+      </c>
+      <c r="K41" t="s">
+        <v>150</v>
+      </c>
+      <c r="L41" t="s">
+        <v>151</v>
+      </c>
+      <c r="M41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>145</v>
-      </c>
-      <c r="I41" t="s">
-        <v>146</v>
-      </c>
-      <c r="J41" t="s">
-        <v>147</v>
-      </c>
-      <c r="K41" t="s">
-        <v>148</v>
-      </c>
-      <c r="L41" t="s">
-        <v>149</v>
-      </c>
-      <c r="M41" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>143</v>
       </c>
       <c r="B42" t="s">
         <v>17</v>
@@ -2885,30 +2880,30 @@
         <v>19</v>
       </c>
       <c r="E42" t="s">
+        <v>153</v>
+      </c>
+      <c r="H42" t="s">
+        <v>147</v>
+      </c>
+      <c r="I42" t="s">
+        <v>148</v>
+      </c>
+      <c r="J42" t="s">
+        <v>149</v>
+      </c>
+      <c r="K42" t="s">
         <v>150</v>
       </c>
-      <c r="H42" t="s">
-        <v>145</v>
-      </c>
-      <c r="I42" t="s">
-        <v>146</v>
-      </c>
-      <c r="J42" t="s">
-        <v>147</v>
-      </c>
-      <c r="K42" t="s">
-        <v>148</v>
-      </c>
       <c r="L42" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M42" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
         <v>17</v>
@@ -2920,100 +2915,100 @@
         <v>19</v>
       </c>
       <c r="E43" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H43" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I43" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J43" t="s">
+        <v>149</v>
+      </c>
+      <c r="K43" t="s">
+        <v>150</v>
+      </c>
+      <c r="L43" t="s">
+        <v>151</v>
+      </c>
+      <c r="M43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" t="s">
         <v>147</v>
       </c>
-      <c r="K43" t="s">
+      <c r="I44" t="s">
         <v>148</v>
       </c>
-      <c r="L43" t="s">
+      <c r="J44" t="s">
         <v>149</v>
       </c>
-      <c r="M43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>155</v>
-      </c>
-      <c r="B44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" t="s">
-        <v>170</v>
-      </c>
-      <c r="E44" t="s">
-        <v>156</v>
-      </c>
-      <c r="H44" t="s">
-        <v>145</v>
-      </c>
-      <c r="I44" t="s">
-        <v>146</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
+        <v>150</v>
+      </c>
+      <c r="L44" t="s">
+        <v>151</v>
+      </c>
+      <c r="M44" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" t="s">
+        <v>162</v>
+      </c>
+      <c r="H45" t="s">
         <v>147</v>
       </c>
-      <c r="K44" t="s">
+      <c r="I45" t="s">
         <v>148</v>
       </c>
-      <c r="L44" t="s">
+      <c r="J45" t="s">
         <v>149</v>
       </c>
-      <c r="M44" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" t="s">
-        <v>170</v>
-      </c>
-      <c r="E45" t="s">
-        <v>158</v>
-      </c>
-      <c r="H45" t="s">
-        <v>145</v>
-      </c>
-      <c r="I45" t="s">
-        <v>146</v>
-      </c>
-      <c r="J45" t="s">
-        <v>147</v>
-      </c>
       <c r="K45" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="L45" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B46" t="s">
         <v>17</v>
@@ -3028,27 +3023,27 @@
         <v>101012</v>
       </c>
       <c r="H46" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J46" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K46" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M46" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B47" t="s">
         <v>17</v>
@@ -3063,27 +3058,27 @@
         <v>101013</v>
       </c>
       <c r="H47" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I47" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J47" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K47" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M47" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
@@ -3098,27 +3093,27 @@
         <v>101015</v>
       </c>
       <c r="H48" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I48" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J48" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K48" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L48" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M48" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B49" t="s">
         <v>17</v>
@@ -3133,27 +3128,27 @@
         <v>101023</v>
       </c>
       <c r="H49" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I49" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J49" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K49" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L49" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M49" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
@@ -3168,29 +3163,27 @@
         <v>101024</v>
       </c>
       <c r="H50" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J50" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K50" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L50" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M50" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P50"/>
-  <sortState ref="A12:P50">
-    <sortCondition ref="A12:A50"/>
-    <sortCondition ref="D12:D50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P50">
+    <sortCondition ref="A1:A50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding updated metadata files (#62)
Co-authored-by: Nilanjana Samanta <nilanjanasamanta@faryabi21.pmacs.upenn.edu>
</commit_message>
<xml_diff>
--- a/assets/metadata/latest/PancDB_ATAC-seq_metadata_2022-06-15.xlsx
+++ b/assets/metadata/latest/PancDB_ATAC-seq_metadata_2022-06-15.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elisabetta\Documents\tmp\PancDB_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilanjanasamanta/Library/CloudStorage/Box-Box/HPAP-IBI/Pancdb-Metadata/current_v3.1.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD0E7E0-FDAA-F943-8ED8-7D1989566827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33810" windowHeight="16665"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33820" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PancDB_ATAC-seq_metadata" sheetId="1" r:id="rId1"/>
@@ -19,14 +20,8 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -326,6 +321,9 @@
     <t>HPAP-035</t>
   </si>
   <si>
+    <t>Islet exocrine cells</t>
+  </si>
+  <si>
     <t>FGC2083</t>
   </si>
   <si>
@@ -341,6 +339,9 @@
     <t>50x50</t>
   </si>
   <si>
+    <t>HPAP-035_exocrine_FGC2083_s_8_1_AGGCAGAA.fastq.gz,HPAP-035_exocrine_FGC2083_s_8_2_AGGCAGAA.fastq.gz</t>
+  </si>
+  <si>
     <t>HPAP-035_alpha_FGC2083_s_8_1_TAAGGCGA.fastq.gz,HPAP-035_alpha_FGC2083_s_8_2_TAAGGCGA.fastq.gz</t>
   </si>
   <si>
@@ -485,6 +486,9 @@
     <t>50x50;50x50;50x50</t>
   </si>
   <si>
+    <t>HPAP-063_exocrine_FGC2163_s_1_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_1_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2163_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_2_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2252_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2252_s_2_2_TAGGCATG.fastq.gz</t>
+  </si>
+  <si>
     <t>99252;99252;103199</t>
   </si>
   <si>
@@ -506,12 +510,18 @@
     <t>99260;99260;103204</t>
   </si>
   <si>
+    <t>HPAP-066_exocrine_FGC2163_s_1_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_1_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2163_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_2_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2252_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2252_s_2_2_GTAGAGGA.fastq.gz</t>
+  </si>
+  <si>
     <t>HPAP-067</t>
   </si>
   <si>
     <t>99263;99263;103206</t>
   </si>
   <si>
+    <t>HPAP-067_exocrine_FGC2163_s_1_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_1_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2163_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_2_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2252_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2252_s_2_2_TGGATCTG.fastq.gz</t>
+  </si>
+  <si>
     <t>HPAP-069</t>
   </si>
   <si>
@@ -543,27 +553,12 @@
   </si>
   <si>
     <t>HPAP-077_beta_FGC2229_s_2_1_GTCGTGAT.fastq.gz,HPAP-077_beta_FGC2229_s_2_2_GTCGTGAT.fastq.gz</t>
-  </si>
-  <si>
-    <t>Islet exocrine cells</t>
-  </si>
-  <si>
-    <t>HPAP-067_exocrine_FGC2163_s_1_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_1_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2163_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2163_s_2_2_TGGATCTG.fastq.gz;HPAP-067_exocrine_FGC2252_s_2_1_TGGATCTG.fastq.gz,HPAP-067_exocrine_FGC2252_s_2_2_TGGATCTG.fastq.gz</t>
-  </si>
-  <si>
-    <t>HPAP-035_exocrine_FGC2083_s_8_1_AGGCAGAA.fastq.gz,HPAP-035_exocrine_FGC2083_s_8_2_AGGCAGAA.fastq.gz</t>
-  </si>
-  <si>
-    <t>HPAP-063_exocrine_FGC2163_s_1_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_1_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2163_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2163_s_2_2_TAGGCATG.fastq.gz;HPAP-063_exocrine_FGC2252_s_2_1_TAGGCATG.fastq.gz,HPAP-063_exocrine_FGC2252_s_2_2_TAGGCATG.fastq.gz</t>
-  </si>
-  <si>
-    <t>HPAP-066_exocrine_FGC2163_s_1_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_1_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2163_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2163_s_2_2_GTAGAGGA.fastq.gz;HPAP-066_exocrine_FGC2252_s_2_1_GTAGAGGA.fastq.gz,HPAP-066_exocrine_FGC2252_s_2_2_GTAGAGGA.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1364,34 +1359,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="64.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="83" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="176.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="176.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1441,7 +1436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1479,9 +1474,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1490,7 +1485,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -1505,10 +1500,10 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="O3" t="s">
         <v>26</v>
@@ -1517,9 +1512,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -1543,10 +1538,10 @@
         <v>23</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O4" t="s">
         <v>26</v>
@@ -1555,9 +1550,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1581,10 +1576,10 @@
         <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="N5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="O5" t="s">
         <v>26</v>
@@ -1593,9 +1588,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1604,7 +1599,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -1619,10 +1614,10 @@
         <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="N6" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="O6" t="s">
         <v>26</v>
@@ -1631,9 +1626,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -1657,10 +1652,10 @@
         <v>23</v>
       </c>
       <c r="M7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O7" t="s">
         <v>26</v>
@@ -1669,9 +1664,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1695,10 +1690,10 @@
         <v>23</v>
       </c>
       <c r="M8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O8" t="s">
         <v>26</v>
@@ -1707,9 +1702,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -1718,36 +1713,33 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="L9" t="s">
+        <v>59</v>
       </c>
       <c r="M9" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -1756,36 +1748,33 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="L10" t="s">
+        <v>59</v>
       </c>
       <c r="M10" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10" t="s">
-        <v>50</v>
-      </c>
-      <c r="O10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -1794,36 +1783,33 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" t="s">
+        <v>66</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="K11" t="s">
-        <v>23</v>
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
+        <v>70</v>
       </c>
       <c r="M11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -1835,30 +1821,30 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="M12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -1869,31 +1855,34 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" t="s">
-        <v>55</v>
+      <c r="F13" t="s">
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="K13" t="s">
-        <v>58</v>
-      </c>
-      <c r="L13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="N13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -1905,7 +1894,7 @@
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
         <v>66</v>
@@ -1923,12 +1912,12 @@
         <v>70</v>
       </c>
       <c r="M14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -1940,7 +1929,7 @@
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
         <v>66</v>
@@ -1958,12 +1947,12 @@
         <v>70</v>
       </c>
       <c r="M15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1974,31 +1963,34 @@
       <c r="D16" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" t="s">
-        <v>66</v>
+      <c r="F16" t="s">
+        <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="J16" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="K16" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="M16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="N16" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -2007,31 +1999,34 @@
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" t="s">
-        <v>66</v>
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="J17" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="K17" t="s">
-        <v>69</v>
-      </c>
-      <c r="L17" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="M17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="N17" t="s">
+        <v>52</v>
+      </c>
+      <c r="O17" t="s">
+        <v>26</v>
+      </c>
+      <c r="P17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -2066,7 +2061,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2101,7 +2096,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -2136,7 +2131,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -2171,7 +2166,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -2206,7 +2201,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -2241,7 +2236,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -2252,31 +2247,31 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
+        <v>97</v>
       </c>
       <c r="E24">
         <v>92020</v>
       </c>
       <c r="H24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M24" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -2293,25 +2288,25 @@
         <v>92018</v>
       </c>
       <c r="H25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -2328,27 +2323,27 @@
         <v>92019</v>
       </c>
       <c r="H26" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
@@ -2360,7 +2355,7 @@
         <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H27" t="s">
         <v>55</v>
@@ -2378,12 +2373,12 @@
         <v>59</v>
       </c>
       <c r="M27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
@@ -2398,27 +2393,27 @@
         <v>92021</v>
       </c>
       <c r="H28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B29" t="s">
         <v>17</v>
@@ -2430,7 +2425,7 @@
         <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H29" t="s">
         <v>55</v>
@@ -2448,12 +2443,12 @@
         <v>59</v>
       </c>
       <c r="M29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>109</v>
       </c>
       <c r="B30" t="s">
         <v>17</v>
@@ -2465,7 +2460,7 @@
         <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H30" t="s">
         <v>55</v>
@@ -2483,12 +2478,12 @@
         <v>59</v>
       </c>
       <c r="M30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
@@ -2503,27 +2498,27 @@
         <v>92024</v>
       </c>
       <c r="H31" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I31" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M31" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -2538,27 +2533,27 @@
         <v>92025</v>
       </c>
       <c r="H32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K32" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
@@ -2570,7 +2565,7 @@
         <v>46</v>
       </c>
       <c r="E33" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H33" t="s">
         <v>66</v>
@@ -2588,12 +2583,12 @@
         <v>70</v>
       </c>
       <c r="M33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
         <v>17</v>
@@ -2605,7 +2600,7 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H34" t="s">
         <v>66</v>
@@ -2623,12 +2618,12 @@
         <v>70</v>
       </c>
       <c r="M34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>120</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -2640,7 +2635,7 @@
         <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H35" t="s">
         <v>66</v>
@@ -2658,12 +2653,12 @@
         <v>70</v>
       </c>
       <c r="M35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
@@ -2675,7 +2670,7 @@
         <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H36" t="s">
         <v>55</v>
@@ -2693,12 +2688,12 @@
         <v>59</v>
       </c>
       <c r="M36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>125</v>
       </c>
       <c r="B37" t="s">
         <v>17</v>
@@ -2710,7 +2705,7 @@
         <v>46</v>
       </c>
       <c r="E37" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H37" t="s">
         <v>55</v>
@@ -2728,12 +2723,12 @@
         <v>59</v>
       </c>
       <c r="M37" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B38" t="s">
         <v>17</v>
@@ -2745,7 +2740,7 @@
         <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H38" t="s">
         <v>55</v>
@@ -2763,12 +2758,12 @@
         <v>59</v>
       </c>
       <c r="M38" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B39" t="s">
         <v>17</v>
@@ -2780,30 +2775,30 @@
         <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H39" t="s">
+        <v>137</v>
+      </c>
+      <c r="I39" t="s">
+        <v>138</v>
+      </c>
+      <c r="J39" t="s">
+        <v>139</v>
+      </c>
+      <c r="K39" t="s">
+        <v>140</v>
+      </c>
+      <c r="L39" t="s">
+        <v>141</v>
+      </c>
+      <c r="M39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>135</v>
-      </c>
-      <c r="I39" t="s">
-        <v>136</v>
-      </c>
-      <c r="J39" t="s">
-        <v>137</v>
-      </c>
-      <c r="K39" t="s">
-        <v>138</v>
-      </c>
-      <c r="L39" t="s">
-        <v>139</v>
-      </c>
-      <c r="M39" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>133</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
@@ -2815,30 +2810,30 @@
         <v>46</v>
       </c>
       <c r="E40" t="s">
+        <v>143</v>
+      </c>
+      <c r="H40" t="s">
+        <v>137</v>
+      </c>
+      <c r="I40" t="s">
+        <v>138</v>
+      </c>
+      <c r="J40" t="s">
+        <v>139</v>
+      </c>
+      <c r="K40" t="s">
+        <v>140</v>
+      </c>
+      <c r="L40" t="s">
         <v>141</v>
       </c>
-      <c r="H40" t="s">
-        <v>135</v>
-      </c>
-      <c r="I40" t="s">
-        <v>136</v>
-      </c>
-      <c r="J40" t="s">
-        <v>137</v>
-      </c>
-      <c r="K40" t="s">
-        <v>138</v>
-      </c>
-      <c r="L40" t="s">
-        <v>139</v>
-      </c>
       <c r="M40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
         <v>17</v>
@@ -2847,33 +2842,33 @@
         <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>170</v>
+        <v>97</v>
       </c>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H41" t="s">
+        <v>147</v>
+      </c>
+      <c r="I41" t="s">
+        <v>148</v>
+      </c>
+      <c r="J41" t="s">
+        <v>149</v>
+      </c>
+      <c r="K41" t="s">
+        <v>150</v>
+      </c>
+      <c r="L41" t="s">
+        <v>151</v>
+      </c>
+      <c r="M41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>145</v>
-      </c>
-      <c r="I41" t="s">
-        <v>146</v>
-      </c>
-      <c r="J41" t="s">
-        <v>147</v>
-      </c>
-      <c r="K41" t="s">
-        <v>148</v>
-      </c>
-      <c r="L41" t="s">
-        <v>149</v>
-      </c>
-      <c r="M41" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>143</v>
       </c>
       <c r="B42" t="s">
         <v>17</v>
@@ -2885,30 +2880,30 @@
         <v>19</v>
       </c>
       <c r="E42" t="s">
+        <v>153</v>
+      </c>
+      <c r="H42" t="s">
+        <v>147</v>
+      </c>
+      <c r="I42" t="s">
+        <v>148</v>
+      </c>
+      <c r="J42" t="s">
+        <v>149</v>
+      </c>
+      <c r="K42" t="s">
         <v>150</v>
       </c>
-      <c r="H42" t="s">
-        <v>145</v>
-      </c>
-      <c r="I42" t="s">
-        <v>146</v>
-      </c>
-      <c r="J42" t="s">
-        <v>147</v>
-      </c>
-      <c r="K42" t="s">
-        <v>148</v>
-      </c>
       <c r="L42" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M42" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
         <v>17</v>
@@ -2920,100 +2915,100 @@
         <v>19</v>
       </c>
       <c r="E43" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H43" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I43" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J43" t="s">
+        <v>149</v>
+      </c>
+      <c r="K43" t="s">
+        <v>150</v>
+      </c>
+      <c r="L43" t="s">
+        <v>151</v>
+      </c>
+      <c r="M43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" t="s">
         <v>147</v>
       </c>
-      <c r="K43" t="s">
+      <c r="I44" t="s">
         <v>148</v>
       </c>
-      <c r="L43" t="s">
+      <c r="J44" t="s">
         <v>149</v>
       </c>
-      <c r="M43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>155</v>
-      </c>
-      <c r="B44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" t="s">
-        <v>170</v>
-      </c>
-      <c r="E44" t="s">
-        <v>156</v>
-      </c>
-      <c r="H44" t="s">
-        <v>145</v>
-      </c>
-      <c r="I44" t="s">
-        <v>146</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
+        <v>150</v>
+      </c>
+      <c r="L44" t="s">
+        <v>151</v>
+      </c>
+      <c r="M44" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" t="s">
+        <v>162</v>
+      </c>
+      <c r="H45" t="s">
         <v>147</v>
       </c>
-      <c r="K44" t="s">
+      <c r="I45" t="s">
         <v>148</v>
       </c>
-      <c r="L44" t="s">
+      <c r="J45" t="s">
         <v>149</v>
       </c>
-      <c r="M44" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" t="s">
-        <v>170</v>
-      </c>
-      <c r="E45" t="s">
-        <v>158</v>
-      </c>
-      <c r="H45" t="s">
-        <v>145</v>
-      </c>
-      <c r="I45" t="s">
-        <v>146</v>
-      </c>
-      <c r="J45" t="s">
-        <v>147</v>
-      </c>
       <c r="K45" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="L45" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B46" t="s">
         <v>17</v>
@@ -3028,27 +3023,27 @@
         <v>101012</v>
       </c>
       <c r="H46" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J46" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K46" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M46" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B47" t="s">
         <v>17</v>
@@ -3063,27 +3058,27 @@
         <v>101013</v>
       </c>
       <c r="H47" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I47" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J47" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K47" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M47" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
@@ -3098,27 +3093,27 @@
         <v>101015</v>
       </c>
       <c r="H48" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I48" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J48" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K48" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L48" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M48" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B49" t="s">
         <v>17</v>
@@ -3133,27 +3128,27 @@
         <v>101023</v>
       </c>
       <c r="H49" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I49" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J49" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K49" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L49" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M49" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B50" t="s">
         <v>17</v>
@@ -3168,29 +3163,27 @@
         <v>101024</v>
       </c>
       <c r="H50" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J50" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="K50" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="L50" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="M50" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P50"/>
-  <sortState ref="A12:P50">
-    <sortCondition ref="A12:A50"/>
-    <sortCondition ref="D12:D50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P50">
+    <sortCondition ref="A1:A50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>